<commit_message>
Save photos to ya disk
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,8 +48,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,19 +425,691 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>42</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Агент</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Компания</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Бренд</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Тип промо</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Бонус</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Условие</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Фото</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Дата создания</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
+        <v>1329793884</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pepsi</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>7UP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>30 руб</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Купить бутылку</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIFzmUMNdyyRpJerOVK_1qM8sXDTofiAAKWzDEbc6JhSLN_7PuaLR4IAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>45190.64162687622</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Русский мех</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>МЕХ</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>gift</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>фапотька</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Купить шубу</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIGE2UMU85tt_Ka9wPY7jwJpR6VtmQRAALCzTEbc6JhSLHGNoNpUzBzAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>45190.73039606585</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Пес-барбос</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Хвостовилялка</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Купить</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIGJWUMWl-CKmfWb3TSSOTz9bCojaaXAALKzzEbTZpZSDQlWlT6NXnBAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>45190.74987269138</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SoftTouch</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ПеринаКул</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Купить 2 шт</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIGNmUMWtqc_hyPTQK2zlRPRu8flGugAAL7zTEbc6JhSEYBVgHpQc52AQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>45190.7512688517</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Fun</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Guy</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>gift</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>By</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>By</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIGRmUMXEsy5AaTRJMWIV_H6fs1Gi6BAAK9zTEb3vpgSKdBLpePcC8vAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>45190.75555517479</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1546318537</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ЭРА</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Эра</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>bonus_tp</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Продай любой ассортимент от 50 тыс рублей в месяц</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIGX2UMcVrpYdyEqARoH07IrB0WOYp6AAIhzjEbc3hhSObPcuJEZ496AQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>45190.81806199338</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Дом клик</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cian</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>bonus_lpr</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>10%</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Одела</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIGfmUNmG4zCOl4zaCXrOeaPjnrguWQAAL9zTEbc6JxSAr0SSLmQ3amAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>45191.69247962826</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ваня</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ремонт</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Никакого</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Поорать на него</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIGj2UNmrrFlQ7NdGzP-TPKH5iJjyFqAAK4zTEb701oSEBlvvUAAVmwrwEAAwIAA3MAAzAE</t>
+        </is>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>45191.69905393606</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Тор</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Хрюкатало</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>gift</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>До жопы слюней</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Купить псяо</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIGumUNnS7hFEPi4JKDy2apfr3jCiVBAAI4zjEbc6JxSJo93lMvS5kOAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>45191.70630134588</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Того</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Реле</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Обе</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIG2mUNn06hqhWCS933pzcNMmzON-Q-AAL9zTEbc6JxSAr0SSLmQ3amAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>45191.71260728829</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Аншлаг</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Киев</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>gift</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Топп</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>План</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIG6WUNoLiInVbSd5ybvAXTbt0h4LpYAAJczjEbc6JxSLR9ZeCBRn0lAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>45191.71680935478</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Лан</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Даст</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>gift</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Тел</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIG-mUNogj2ulRKXQM0ijHvr1HeDugvAAL9zTEbc6JxSAr0SSLmQ3amAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>45191.72068371337</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>iugo</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>hfgiv</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>uytfiuky</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIHMGUSbykYRPErF_f1vsAeWWSXtXHPAALzyDEbAtWYSMtnAdWWh0aBAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>45195.36260482792</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ertgwert</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>wergwertg</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>gift</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>wrtb</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>wreb</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIHRmUScBwWiJinqj7WF4bU49DvjL6cAAL-yDEbAtWYSGLIoWsyRzMgAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>45195.36535166229</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Бобик</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Добик</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>gift</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Лобик</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Мобик</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIHa2USj3SbqdAx2fLg46d0LUvUosxFAALdzzEbpneISK4YGBNCA6q5AQADAgADcwADMAQ</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>45195.45822453291</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>sdfghjk</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>dfghjk</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>jghkgj</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIHumUSzVEK_TyK0XvNlcLhe4hmd1kJAALuyzEbAtWYSGYa1ePozhaCAQADAgADeQADMAQ</t>
+        </is>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>45195.64151998855</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1329793884</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>typ</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>jni</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>jon</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAIHyWUSzd4az7-nkhGj6uDM4vflzLwyAALuyzEbAtWYSGYa1ePozhaCAQADAgADeQADMAQ</t>
+        </is>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>45195.64316129083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>